<commit_message>
02.07.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/July/Others/Requisition of Tulip-2.xlsx
+++ b/July/Others/Requisition of Tulip-2.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="105">
   <si>
     <t>Model Name</t>
   </si>
@@ -287,9 +287,6 @@
   </si>
   <si>
     <t>Black_Red</t>
-  </si>
-  <si>
-    <t>Gold/Black</t>
   </si>
   <si>
     <t>B60</t>
@@ -349,10 +346,16 @@
     <t>D52+</t>
   </si>
   <si>
-    <t>30.06.19</t>
-  </si>
-  <si>
     <t>Gold &amp; Black</t>
+  </si>
+  <si>
+    <t>Black/Gold</t>
+  </si>
+  <si>
+    <t>Black/Black_Blue</t>
+  </si>
+  <si>
+    <t>02.07.19</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1015,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomRight" activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1027,7 +1030,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" ht="12.75">
       <c r="A1" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -1055,7 +1058,7 @@
         <v>27</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="6" customFormat="1" ht="12.75">
@@ -1088,7 +1091,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" hidden="1">
@@ -1121,7 +1124,7 @@
     </row>
     <row r="8" spans="1:5" ht="15" hidden="1">
       <c r="A8" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" s="9">
         <v>760.9</v>
@@ -1132,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" hidden="1">
@@ -1153,7 +1156,7 @@
     </row>
     <row r="10" spans="1:5" ht="15" hidden="1">
       <c r="A10" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="9">
         <v>896.24</v>
@@ -1197,17 +1200,19 @@
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:5" ht="15" hidden="1">
+    <row r="13" spans="1:5" ht="15">
       <c r="A13" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="9">
         <v>901.24749999999995</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="8">
+        <v>15</v>
+      </c>
       <c r="D13" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13518.7125</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>84</v>
@@ -1226,7 +1231,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
@@ -1289,22 +1294,20 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5" ht="15" hidden="1">
       <c r="A19" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B19" s="9">
         <v>1159.8900000000001</v>
       </c>
-      <c r="C19" s="8">
-        <v>60</v>
-      </c>
+      <c r="C19" s="8"/>
       <c r="D19" s="10">
         <f>B19*C19</f>
-        <v>69593.400000000009</v>
+        <v>0</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" hidden="1">
@@ -1351,14 +1354,12 @@
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" ht="15">
+    <row r="23" spans="1:5" ht="15" hidden="1">
       <c r="A23" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B23" s="9"/>
-      <c r="C23" s="8">
-        <v>40</v>
-      </c>
+      <c r="C23" s="8"/>
       <c r="D23" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1397,20 +1398,22 @@
       </c>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" ht="15" hidden="1">
+    <row r="26" spans="1:5" ht="15">
       <c r="A26" s="8" t="s">
         <v>75</v>
       </c>
       <c r="B26" s="9">
         <v>2710.76</v>
       </c>
-      <c r="C26" s="8"/>
+      <c r="C26" s="8">
+        <v>3</v>
+      </c>
       <c r="D26" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8132.2800000000007</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" hidden="1">
@@ -1483,20 +1486,22 @@
       </c>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" ht="15" hidden="1">
+    <row r="32" spans="1:5" ht="15">
       <c r="A32" s="8" t="s">
         <v>77</v>
       </c>
       <c r="B32" s="9">
         <v>5793.4475000000002</v>
       </c>
-      <c r="C32" s="8"/>
+      <c r="C32" s="8">
+        <v>6</v>
+      </c>
       <c r="D32" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>34760.684999999998</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" hidden="1">
@@ -1540,7 +1545,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" hidden="1">
@@ -1643,17 +1648,19 @@
       </c>
       <c r="E42" s="8"/>
     </row>
-    <row r="43" spans="1:5" ht="15" hidden="1">
+    <row r="43" spans="1:5" ht="15">
       <c r="A43" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B43" s="9">
         <v>1053.6275000000001</v>
       </c>
-      <c r="C43" s="8"/>
+      <c r="C43" s="8">
+        <v>10</v>
+      </c>
       <c r="D43" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10536.275000000001</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>89</v>
@@ -1673,17 +1680,19 @@
       </c>
       <c r="E44" s="8"/>
     </row>
-    <row r="45" spans="1:5" ht="15" hidden="1">
+    <row r="45" spans="1:5" ht="15">
       <c r="A45" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B45" s="9">
         <v>1092.7249999999999</v>
       </c>
-      <c r="C45" s="8"/>
+      <c r="C45" s="8">
+        <v>15</v>
+      </c>
       <c r="D45" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16390.875</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>84</v>
@@ -1714,17 +1723,19 @@
       <c r="D47" s="10"/>
       <c r="E47" s="8"/>
     </row>
-    <row r="48" spans="1:5" ht="15" hidden="1">
+    <row r="48" spans="1:5" ht="15">
       <c r="A48" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B48" s="9">
         <v>1077.6875</v>
       </c>
-      <c r="C48" s="8"/>
+      <c r="C48" s="8">
+        <v>15</v>
+      </c>
       <c r="D48" s="10">
         <f>B48*C48</f>
-        <v>0</v>
+        <v>16165.3125</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>84</v>
@@ -1872,17 +1883,19 @@
       </c>
       <c r="E58" s="8"/>
     </row>
-    <row r="59" spans="1:5" ht="15" hidden="1">
+    <row r="59" spans="1:5" ht="15">
       <c r="A59" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B59" s="9">
         <v>4896.21</v>
       </c>
-      <c r="C59" s="8"/>
+      <c r="C59" s="8">
+        <v>3</v>
+      </c>
       <c r="D59" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>14688.630000000001</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>88</v>
@@ -1902,33 +1915,41 @@
       </c>
       <c r="E60" s="8"/>
     </row>
-    <row r="61" spans="1:5" ht="15" hidden="1">
+    <row r="61" spans="1:5" ht="15">
       <c r="A61" s="8" t="s">
         <v>64</v>
       </c>
       <c r="B61" s="9">
         <v>4973.4025000000001</v>
       </c>
-      <c r="C61" s="8"/>
+      <c r="C61" s="8">
+        <v>2</v>
+      </c>
       <c r="D61" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E61" s="8"/>
-    </row>
-    <row r="62" spans="1:5" ht="15" hidden="1">
+        <v>9946.8050000000003</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15">
       <c r="A62" s="8" t="s">
         <v>83</v>
       </c>
       <c r="B62" s="9">
         <v>4701.7299999999996</v>
       </c>
-      <c r="C62" s="8"/>
+      <c r="C62" s="8">
+        <v>6</v>
+      </c>
       <c r="D62" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E62" s="8"/>
+        <v>28210.379999999997</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="63" spans="1:5" ht="15" hidden="1">
       <c r="A63" s="8" t="s">
@@ -2000,17 +2021,19 @@
       </c>
       <c r="E67" s="8"/>
     </row>
-    <row r="68" spans="1:5" ht="15" hidden="1">
+    <row r="68" spans="1:5" ht="15">
       <c r="A68" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B68" s="9">
         <v>4389.9475000000002</v>
       </c>
-      <c r="C68" s="8"/>
+      <c r="C68" s="8">
+        <v>6</v>
+      </c>
       <c r="D68" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>26339.685000000001</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>86</v>
@@ -2072,37 +2095,45 @@
       </c>
       <c r="E72" s="8"/>
     </row>
-    <row r="73" spans="1:5" ht="15" hidden="1">
+    <row r="73" spans="1:5" ht="15">
       <c r="A73" s="8" t="s">
         <v>62</v>
       </c>
       <c r="B73" s="9">
         <v>3979.9250000000002</v>
       </c>
-      <c r="C73" s="8"/>
+      <c r="C73" s="8">
+        <v>2</v>
+      </c>
       <c r="D73" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E73" s="8"/>
-    </row>
-    <row r="74" spans="1:5" ht="15" hidden="1">
+        <v>7959.85</v>
+      </c>
+      <c r="E73" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15">
       <c r="A74" s="8" t="s">
         <v>73</v>
       </c>
       <c r="B74" s="9">
         <v>4115.2624999999998</v>
       </c>
-      <c r="C74" s="8"/>
+      <c r="C74" s="8">
+        <v>2</v>
+      </c>
       <c r="D74" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E74" s="8"/>
+        <v>8230.5249999999996</v>
+      </c>
+      <c r="E74" s="8" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="75" spans="1:5" ht="15" hidden="1">
       <c r="A75" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B75" s="9">
         <v>1219.04</v>
@@ -2137,11 +2168,11 @@
       <c r="B77" s="37"/>
       <c r="C77" s="24">
         <f>SUM(C5:C76)</f>
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="D77" s="25">
         <f>SUM(D5:D76)</f>
-        <v>69593.400000000009</v>
+        <v>194880.01500000001</v>
       </c>
       <c r="E77" s="24"/>
     </row>
@@ -2200,7 +2231,7 @@
         <v>22</v>
       </c>
       <c r="C84" s="29">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="D84" s="8"/>
       <c r="E84" s="14"/>
@@ -2248,7 +2279,7 @@
       </c>
       <c r="C89" s="30">
         <f>SUM(C83:C88)</f>
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="D89" s="20"/>
       <c r="E89" s="14"/>

</xml_diff>